<commit_message>
Added new algorithm, ESMod, to evolution.py
</commit_message>
<xml_diff>
--- a/tables/table1_dim10.xlsx
+++ b/tables/table1_dim10.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Best</t>
   </si>
@@ -35,22 +35,7 @@
     <t>Success Rate</t>
   </si>
   <si>
-    <t>F14</t>
-  </si>
-  <si>
-    <t>Fc1</t>
-  </si>
-  <si>
-    <t>Fc2</t>
-  </si>
-  <si>
-    <t>Fc6</t>
-  </si>
-  <si>
-    <t>Fc7</t>
-  </si>
-  <si>
-    <t>Fc9</t>
+    <t>Fnc</t>
   </si>
 </sst>
 </file>
@@ -399,7 +384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,136 +417,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1396</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.625</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3526</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.3298</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s"/>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1981.8553</v>
-      </c>
-      <c r="C3" t="n">
-        <v>243109.8101</v>
-      </c>
-      <c r="D3" t="n">
-        <v>71750.2962</v>
-      </c>
-      <c r="E3" t="n">
-        <v>91073.74830000001</v>
-      </c>
-      <c r="F3" t="n">
-        <v>72900.0716</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.0615</v>
-      </c>
-      <c r="C4" t="n">
-        <v>11722.6875</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3855.6945</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4191.4865</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3261.1716</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2.7544</v>
-      </c>
-      <c r="C5" t="n">
-        <v>9.255800000000001</v>
-      </c>
-      <c r="D5" t="n">
-        <v>5.4755</v>
-      </c>
-      <c r="E5" t="n">
-        <v>5.473</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.6991</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.0271</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2.3425</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.209</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.3785</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.4235</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="n">
-        <v>12.9345</v>
-      </c>
-      <c r="C7" t="n">
-        <v>61.6872</v>
-      </c>
-      <c r="D7" t="n">
-        <v>31.8386</v>
-      </c>
-      <c r="E7" t="n">
-        <v>32.08</v>
-      </c>
-      <c r="F7" t="n">
-        <v>12.2439</v>
-      </c>
-      <c r="G7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated make_tables for variable population size algorithms
</commit_message>
<xml_diff>
--- a/tables/table1_dim10.xlsx
+++ b/tables/table1_dim10.xlsx
@@ -35,7 +35,7 @@
     <t>Success Rate</t>
   </si>
   <si>
-    <t>Fnc</t>
+    <t>Fc2</t>
   </si>
 </sst>
 </file>
@@ -417,18 +417,20 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3.7763</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>11707.8297</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>3787.6483</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s"/>
+        <v>4276.1202</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3903.5288</v>
+      </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>

</xml_diff>